<commit_message>
Gantt chart milestones established. Main
Finished what need doing today. 2/05/2024
</commit_message>
<xml_diff>
--- a/Agile Gantt chart.xlsx
+++ b/Agile Gantt chart.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCFAED0C-4FE9-4DE3-A9CB-67435695739C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA95D447-CDB4-4D9B-BBF2-36DD8ED30FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28665" yWindow="3465" windowWidth="18900" windowHeight="11055" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="415" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="55">
   <si>
     <t>Task 3</t>
   </si>
@@ -184,14 +184,68 @@
 •  Add the day you started your project in the Start Date. 
 •  Finish your calculations by filling in the number of days you need to complete your project in the No. of Days field. </t>
   </si>
+  <si>
+    <t>Chinese Palace - Website</t>
+  </si>
+  <si>
+    <t>JZTC</t>
+  </si>
+  <si>
+    <t>Joemama</t>
+  </si>
+  <si>
+    <t>Complete stakeholder  register</t>
+  </si>
+  <si>
+    <t>Split team into groups</t>
+  </si>
+  <si>
+    <t>Complete personas</t>
+  </si>
+  <si>
+    <t>Complete persona reviews</t>
+  </si>
+  <si>
+    <t>Complete group meeting report</t>
+  </si>
+  <si>
+    <t>Complete iteration 2  progress report</t>
+  </si>
+  <si>
+    <t>Complete Iteration 1 progress report</t>
+  </si>
+  <si>
+    <t>Complete resources needs documentation</t>
+  </si>
+  <si>
+    <t>Complete gantt chart</t>
+  </si>
+  <si>
+    <t>Complete iteration 2 group meeting report</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Jo, Zoe, Tainui, Cairo</t>
+  </si>
+  <si>
+    <t>Complete iteration 3 progress report</t>
+  </si>
+  <si>
+    <t>Establish project times and devlierables using a gantt chart</t>
+  </si>
+  <si>
+    <t>Migrate task management from Google drive to Github repositories</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="d"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="d"/>
   </numFmts>
   <fonts count="34" x14ac:knownFonts="1">
     <font>
@@ -761,7 +815,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
@@ -822,10 +876,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -887,13 +941,13 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -971,7 +1025,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1081,32 +1135,32 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="14" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="14" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="14" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="14" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2427,7 +2481,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$C$7" horiz="1" max="365" page="2"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$C$7" horiz="1" max="365" page="2" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2695,7 +2749,7 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6E47A83D-ACD7-4EB6-9B84-5195E813945E}" name="Milestone description" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{6E47A83D-ACD7-4EB6-9B84-5195E813945E}" name="Complete Iteration 1 progress report" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{529EEF64-D037-4ACF-8CA4-0C10FE2D1FBB}" name="Category" dataDxfId="19"/>
     <tableColumn id="3" xr3:uid="{711D01BA-2785-403A-9636-CCC7E2ADA584}" name="Assigned to" dataDxfId="18"/>
     <tableColumn id="4" xr3:uid="{62B00BEF-16BE-4692-B5E2-F287F680F2C1}" name="Progress"/>
@@ -3004,7 +3058,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3487,7 +3543,7 @@
       </c>
       <c r="C6" s="90" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">IFERROR(IF(MIN(Milestones4352[Start])=0,TODAY(),B11(Milestones4352[Start])),TODAY())</f>
-        <v>44407</v>
+        <v>45414</v>
       </c>
       <c r="D6" s="91"/>
       <c r="E6" s="84"/>
@@ -3496,7 +3552,7 @@
       <c r="H6" s="84"/>
       <c r="I6" s="109" t="str">
         <f ca="1">TEXT(I7,"mmmm")</f>
-        <v>July</v>
+        <v>May</v>
       </c>
       <c r="J6" s="109"/>
       <c r="K6" s="109"/>
@@ -3506,7 +3562,7 @@
       <c r="O6" s="109"/>
       <c r="P6" s="109" t="str">
         <f ca="1">IF(TEXT(P7,"mmmm")=I6,"",TEXT(P7,"mmmm"))</f>
-        <v>August</v>
+        <v/>
       </c>
       <c r="Q6" s="109"/>
       <c r="R6" s="109"/>
@@ -3546,7 +3602,7 @@
       <c r="AQ6" s="109"/>
       <c r="AR6" s="109" t="str">
         <f ca="1">IF(OR(TEXT(AR7,"mmmm")=AK6,TEXT(AR7,"mmmm")=AD6,TEXT(AR7,"mmmm")=W6,TEXT(AR7,"mmmm")=P6),"",TEXT(AR7,"mmmm"))</f>
-        <v>September</v>
+        <v>June</v>
       </c>
       <c r="AS6" s="109"/>
       <c r="AT6" s="109"/>
@@ -3591,227 +3647,227 @@
       <c r="H7" s="94"/>
       <c r="I7" s="116">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>44408</v>
+        <v>45415</v>
       </c>
       <c r="J7" s="117">
         <f ca="1">I7+1</f>
-        <v>44409</v>
+        <v>45416</v>
       </c>
       <c r="K7" s="117">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>44410</v>
+        <v>45417</v>
       </c>
       <c r="L7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44411</v>
+        <v>45418</v>
       </c>
       <c r="M7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>45419</v>
       </c>
       <c r="N7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44413</v>
+        <v>45420</v>
       </c>
       <c r="O7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44414</v>
+        <v>45421</v>
       </c>
       <c r="P7" s="117">
         <f ca="1">O7+1</f>
-        <v>44415</v>
+        <v>45422</v>
       </c>
       <c r="Q7" s="117">
         <f ca="1">P7+1</f>
-        <v>44416</v>
+        <v>45423</v>
       </c>
       <c r="R7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44417</v>
+        <v>45424</v>
       </c>
       <c r="S7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44418</v>
+        <v>45425</v>
       </c>
       <c r="T7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44419</v>
+        <v>45426</v>
       </c>
       <c r="U7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44420</v>
+        <v>45427</v>
       </c>
       <c r="V7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44421</v>
+        <v>45428</v>
       </c>
       <c r="W7" s="117">
         <f ca="1">V7+1</f>
-        <v>44422</v>
+        <v>45429</v>
       </c>
       <c r="X7" s="117">
         <f ca="1">W7+1</f>
-        <v>44423</v>
+        <v>45430</v>
       </c>
       <c r="Y7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44424</v>
+        <v>45431</v>
       </c>
       <c r="Z7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44425</v>
+        <v>45432</v>
       </c>
       <c r="AA7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44426</v>
+        <v>45433</v>
       </c>
       <c r="AB7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44427</v>
+        <v>45434</v>
       </c>
       <c r="AC7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44428</v>
+        <v>45435</v>
       </c>
       <c r="AD7" s="117">
         <f ca="1">AC7+1</f>
-        <v>44429</v>
+        <v>45436</v>
       </c>
       <c r="AE7" s="117">
         <f ca="1">AD7+1</f>
-        <v>44430</v>
+        <v>45437</v>
       </c>
       <c r="AF7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44431</v>
+        <v>45438</v>
       </c>
       <c r="AG7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44432</v>
+        <v>45439</v>
       </c>
       <c r="AH7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44433</v>
+        <v>45440</v>
       </c>
       <c r="AI7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44434</v>
+        <v>45441</v>
       </c>
       <c r="AJ7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44435</v>
+        <v>45442</v>
       </c>
       <c r="AK7" s="117">
         <f ca="1">AJ7+1</f>
-        <v>44436</v>
+        <v>45443</v>
       </c>
       <c r="AL7" s="117">
         <f ca="1">AK7+1</f>
-        <v>44437</v>
+        <v>45444</v>
       </c>
       <c r="AM7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44438</v>
+        <v>45445</v>
       </c>
       <c r="AN7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44439</v>
+        <v>45446</v>
       </c>
       <c r="AO7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44440</v>
+        <v>45447</v>
       </c>
       <c r="AP7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44441</v>
+        <v>45448</v>
       </c>
       <c r="AQ7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44442</v>
+        <v>45449</v>
       </c>
       <c r="AR7" s="117">
         <f ca="1">AQ7+1</f>
-        <v>44443</v>
+        <v>45450</v>
       </c>
       <c r="AS7" s="117">
         <f ca="1">AR7+1</f>
-        <v>44444</v>
+        <v>45451</v>
       </c>
       <c r="AT7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44445</v>
+        <v>45452</v>
       </c>
       <c r="AU7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44446</v>
+        <v>45453</v>
       </c>
       <c r="AV7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44447</v>
+        <v>45454</v>
       </c>
       <c r="AW7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44448</v>
+        <v>45455</v>
       </c>
       <c r="AX7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44449</v>
+        <v>45456</v>
       </c>
       <c r="AY7" s="117">
         <f ca="1">AX7+1</f>
-        <v>44450</v>
+        <v>45457</v>
       </c>
       <c r="AZ7" s="117">
         <f ca="1">AY7+1</f>
-        <v>44451</v>
+        <v>45458</v>
       </c>
       <c r="BA7" s="117">
         <f t="shared" ref="BA7:BE7" ca="1" si="1">AZ7+1</f>
-        <v>44452</v>
+        <v>45459</v>
       </c>
       <c r="BB7" s="117">
         <f t="shared" ca="1" si="1"/>
-        <v>44453</v>
+        <v>45460</v>
       </c>
       <c r="BC7" s="117">
         <f t="shared" ca="1" si="1"/>
-        <v>44454</v>
+        <v>45461</v>
       </c>
       <c r="BD7" s="117">
         <f t="shared" ca="1" si="1"/>
-        <v>44455</v>
+        <v>45462</v>
       </c>
       <c r="BE7" s="118">
         <f t="shared" ca="1" si="1"/>
-        <v>44456</v>
+        <v>45463</v>
       </c>
       <c r="BF7" s="117">
         <f ca="1">BE7+1</f>
-        <v>44457</v>
+        <v>45464</v>
       </c>
       <c r="BG7" s="117">
         <f ca="1">BF7+1</f>
-        <v>44458</v>
+        <v>45465</v>
       </c>
       <c r="BH7" s="117">
         <f t="shared" ref="BH7:BL7" ca="1" si="2">BG7+1</f>
-        <v>44459</v>
+        <v>45466</v>
       </c>
       <c r="BI7" s="117">
         <f t="shared" ca="1" si="2"/>
-        <v>44460</v>
+        <v>45467</v>
       </c>
       <c r="BJ7" s="117">
         <f t="shared" ca="1" si="2"/>
-        <v>44461</v>
+        <v>45468</v>
       </c>
       <c r="BK7" s="117">
         <f t="shared" ca="1" si="2"/>
-        <v>44462</v>
+        <v>45469</v>
       </c>
       <c r="BL7" s="118">
         <f t="shared" ca="1" si="2"/>
-        <v>44463</v>
+        <v>45470</v>
       </c>
       <c r="BM7" s="99"/>
     </row>
@@ -3905,7 +3961,7 @@
       <c r="H9" s="105"/>
       <c r="I9" s="124" t="str">
         <f t="shared" ref="I9:BL9" ca="1" si="3">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="J9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3913,27 +3969,27 @@
       </c>
       <c r="K9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="L9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="M9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="N9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="O9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="P9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="Q9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3941,27 +3997,27 @@
       </c>
       <c r="R9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="S9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="T9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="U9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="V9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="W9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="X9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3969,27 +4025,27 @@
       </c>
       <c r="Y9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="Z9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AA9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="AB9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="AC9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AD9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AE9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3997,27 +4053,27 @@
       </c>
       <c r="AF9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AG9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AH9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="AI9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="AJ9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AK9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AL9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4025,27 +4081,27 @@
       </c>
       <c r="AM9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AN9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AO9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="AP9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="AQ9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AR9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AS9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4053,27 +4109,27 @@
       </c>
       <c r="AT9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AU9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AV9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="AW9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="AX9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AY9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AZ9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4081,27 +4137,27 @@
       </c>
       <c r="BA9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BB9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="BC9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="BD9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="BE9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="BF9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="BG9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4109,23 +4165,23 @@
       </c>
       <c r="BH9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BI9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="BJ9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="BK9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="BL9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="BM9" s="99"/>
     </row>
@@ -4449,7 +4505,7 @@
       </c>
       <c r="F12" s="69">
         <f ca="1">TODAY()</f>
-        <v>44407</v>
+        <v>45414</v>
       </c>
       <c r="G12" s="70">
         <v>3</v>
@@ -4693,7 +4749,7 @@
       <c r="E13" s="68"/>
       <c r="F13" s="69">
         <f ca="1">TODAY()+5</f>
-        <v>44412</v>
+        <v>45419</v>
       </c>
       <c r="G13" s="70">
         <v>1</v>
@@ -4939,7 +4995,7 @@
       </c>
       <c r="F14" s="69">
         <f ca="1">F12-3</f>
-        <v>44404</v>
+        <v>45411</v>
       </c>
       <c r="G14" s="70">
         <v>10</v>
@@ -5183,7 +5239,7 @@
       <c r="E15" s="68"/>
       <c r="F15" s="69">
         <f ca="1">F12+20</f>
-        <v>44427</v>
+        <v>45434</v>
       </c>
       <c r="G15" s="70">
         <v>1</v>
@@ -5429,7 +5485,7 @@
       </c>
       <c r="F16" s="69">
         <f ca="1">F12+6</f>
-        <v>44413</v>
+        <v>45420</v>
       </c>
       <c r="G16" s="70">
         <v>6</v>
@@ -5912,7 +5968,7 @@
       </c>
       <c r="F18" s="69">
         <f ca="1">F12+6</f>
-        <v>44413</v>
+        <v>45420</v>
       </c>
       <c r="G18" s="70">
         <v>13</v>
@@ -6158,7 +6214,7 @@
       </c>
       <c r="F19" s="69">
         <f ca="1">F18+2</f>
-        <v>44415</v>
+        <v>45422</v>
       </c>
       <c r="G19" s="70">
         <v>9</v>
@@ -6404,7 +6460,7 @@
       </c>
       <c r="F20" s="69">
         <f ca="1">F19+5</f>
-        <v>44420</v>
+        <v>45427</v>
       </c>
       <c r="G20" s="70">
         <v>11</v>
@@ -6648,7 +6704,7 @@
       <c r="E21" s="68"/>
       <c r="F21" s="69">
         <f ca="1">F20+2</f>
-        <v>44422</v>
+        <v>45429</v>
       </c>
       <c r="G21" s="70">
         <v>1</v>
@@ -6890,7 +6946,7 @@
       <c r="E22" s="68"/>
       <c r="F22" s="69">
         <f ca="1">F21+1</f>
-        <v>44423</v>
+        <v>45430</v>
       </c>
       <c r="G22" s="70">
         <v>24</v>
@@ -7371,7 +7427,7 @@
       <c r="E24" s="68"/>
       <c r="F24" s="69">
         <f ca="1">F12+15</f>
-        <v>44422</v>
+        <v>45429</v>
       </c>
       <c r="G24" s="70">
         <v>4</v>
@@ -7615,7 +7671,7 @@
       <c r="E25" s="68"/>
       <c r="F25" s="69">
         <f ca="1">F24+3</f>
-        <v>44425</v>
+        <v>45432</v>
       </c>
       <c r="G25" s="70">
         <v>14</v>
@@ -7859,7 +7915,7 @@
       <c r="E26" s="68"/>
       <c r="F26" s="69">
         <f ca="1">F25+15</f>
-        <v>44440</v>
+        <v>45447</v>
       </c>
       <c r="G26" s="70">
         <v>6</v>
@@ -8103,7 +8159,7 @@
       <c r="E27" s="68"/>
       <c r="F27" s="69">
         <f ca="1">F21+22</f>
-        <v>44444</v>
+        <v>45451</v>
       </c>
       <c r="G27" s="70">
         <v>3</v>
@@ -8347,7 +8403,7 @@
       <c r="E28" s="68"/>
       <c r="F28" s="69">
         <f ca="1">F16</f>
-        <v>44413</v>
+        <v>45420</v>
       </c>
       <c r="G28" s="70">
         <v>19</v>
@@ -8826,7 +8882,7 @@
       <c r="E30" s="68"/>
       <c r="F30" s="69">
         <f ca="1">F27+3</f>
-        <v>44447</v>
+        <v>45454</v>
       </c>
       <c r="G30" s="70">
         <v>15</v>
@@ -9068,7 +9124,7 @@
       <c r="E31" s="68"/>
       <c r="F31" s="69">
         <f ca="1">F30+14</f>
-        <v>44461</v>
+        <v>45468</v>
       </c>
       <c r="G31" s="70">
         <v>5</v>
@@ -9312,7 +9368,7 @@
       <c r="E32" s="68"/>
       <c r="F32" s="69">
         <f ca="1">F31+42</f>
-        <v>44503</v>
+        <v>45510</v>
       </c>
       <c r="G32" s="70">
         <v>1</v>
@@ -10538,12 +10594,14 @@
   </sheetPr>
   <dimension ref="A1:BP38"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="C4" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" style="12" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" style="12" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" style="12" customWidth="1"/>
@@ -10559,7 +10617,7 @@
     <row r="2" spans="1:68" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="152" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="C2" s="152"/>
       <c r="D2" s="152"/>
@@ -10695,7 +10753,7 @@
     <row r="4" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="62" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C4" s="57"/>
       <c r="D4" s="58"/>
@@ -10776,7 +10834,7 @@
     <row r="5" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="63" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="59"/>
@@ -10849,7 +10907,7 @@
       </c>
       <c r="C6" s="39" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">IFERROR(IF(MIN(Milestones435[Start])=0,TODAY(),B11(Milestones435[Start])),TODAY())</f>
-        <v>44407</v>
+        <v>45414</v>
       </c>
       <c r="D6" s="60"/>
       <c r="E6" s="35"/>
@@ -10858,7 +10916,7 @@
       <c r="H6" s="32"/>
       <c r="I6" s="112" t="str">
         <f ca="1">TEXT(I7,"mmmm")</f>
-        <v>July</v>
+        <v>May</v>
       </c>
       <c r="J6" s="112"/>
       <c r="K6" s="112"/>
@@ -10868,7 +10926,7 @@
       <c r="O6" s="112"/>
       <c r="P6" s="112" t="str">
         <f ca="1">IF(TEXT(P7,"mmmm")=I6,"",TEXT(P7,"mmmm"))</f>
-        <v>August</v>
+        <v/>
       </c>
       <c r="Q6" s="112"/>
       <c r="R6" s="112"/>
@@ -10908,7 +10966,7 @@
       <c r="AQ6" s="112"/>
       <c r="AR6" s="112" t="str">
         <f ca="1">IF(OR(TEXT(AR7,"mmmm")=AK6,TEXT(AR7,"mmmm")=AD6,TEXT(AR7,"mmmm")=W6,TEXT(AR7,"mmmm")=P6),"",TEXT(AR7,"mmmm"))</f>
-        <v>September</v>
+        <v>June</v>
       </c>
       <c r="AS6" s="112"/>
       <c r="AT6" s="112"/>
@@ -10944,7 +11002,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="59"/>
       <c r="E7" s="32"/>
@@ -10953,227 +11011,227 @@
       <c r="H7" s="38"/>
       <c r="I7" s="114">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>44408</v>
+        <v>45414</v>
       </c>
       <c r="J7" s="19">
         <f ca="1">I7+1</f>
-        <v>44409</v>
+        <v>45415</v>
       </c>
       <c r="K7" s="19">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>44410</v>
+        <v>45416</v>
       </c>
       <c r="L7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44411</v>
+        <v>45417</v>
       </c>
       <c r="M7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>45418</v>
       </c>
       <c r="N7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44413</v>
+        <v>45419</v>
       </c>
       <c r="O7" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>44414</v>
+        <v>45420</v>
       </c>
       <c r="P7" s="19">
         <f ca="1">O7+1</f>
-        <v>44415</v>
+        <v>45421</v>
       </c>
       <c r="Q7" s="19">
         <f ca="1">P7+1</f>
-        <v>44416</v>
+        <v>45422</v>
       </c>
       <c r="R7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44417</v>
+        <v>45423</v>
       </c>
       <c r="S7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44418</v>
+        <v>45424</v>
       </c>
       <c r="T7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44419</v>
+        <v>45425</v>
       </c>
       <c r="U7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44420</v>
+        <v>45426</v>
       </c>
       <c r="V7" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>44421</v>
+        <v>45427</v>
       </c>
       <c r="W7" s="19">
         <f ca="1">V7+1</f>
-        <v>44422</v>
+        <v>45428</v>
       </c>
       <c r="X7" s="19">
         <f ca="1">W7+1</f>
-        <v>44423</v>
+        <v>45429</v>
       </c>
       <c r="Y7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44424</v>
+        <v>45430</v>
       </c>
       <c r="Z7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44425</v>
+        <v>45431</v>
       </c>
       <c r="AA7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44426</v>
+        <v>45432</v>
       </c>
       <c r="AB7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44427</v>
+        <v>45433</v>
       </c>
       <c r="AC7" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>44428</v>
+        <v>45434</v>
       </c>
       <c r="AD7" s="19">
         <f ca="1">AC7+1</f>
-        <v>44429</v>
+        <v>45435</v>
       </c>
       <c r="AE7" s="19">
         <f ca="1">AD7+1</f>
-        <v>44430</v>
+        <v>45436</v>
       </c>
       <c r="AF7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44431</v>
+        <v>45437</v>
       </c>
       <c r="AG7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44432</v>
+        <v>45438</v>
       </c>
       <c r="AH7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44433</v>
+        <v>45439</v>
       </c>
       <c r="AI7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44434</v>
+        <v>45440</v>
       </c>
       <c r="AJ7" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>44435</v>
+        <v>45441</v>
       </c>
       <c r="AK7" s="19">
         <f ca="1">AJ7+1</f>
-        <v>44436</v>
+        <v>45442</v>
       </c>
       <c r="AL7" s="19">
         <f ca="1">AK7+1</f>
-        <v>44437</v>
+        <v>45443</v>
       </c>
       <c r="AM7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44438</v>
+        <v>45444</v>
       </c>
       <c r="AN7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44439</v>
+        <v>45445</v>
       </c>
       <c r="AO7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44440</v>
+        <v>45446</v>
       </c>
       <c r="AP7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44441</v>
+        <v>45447</v>
       </c>
       <c r="AQ7" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>44442</v>
+        <v>45448</v>
       </c>
       <c r="AR7" s="19">
         <f ca="1">AQ7+1</f>
-        <v>44443</v>
+        <v>45449</v>
       </c>
       <c r="AS7" s="19">
         <f ca="1">AR7+1</f>
-        <v>44444</v>
+        <v>45450</v>
       </c>
       <c r="AT7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44445</v>
+        <v>45451</v>
       </c>
       <c r="AU7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44446</v>
+        <v>45452</v>
       </c>
       <c r="AV7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44447</v>
+        <v>45453</v>
       </c>
       <c r="AW7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44448</v>
+        <v>45454</v>
       </c>
       <c r="AX7" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>44449</v>
+        <v>45455</v>
       </c>
       <c r="AY7" s="19">
         <f ca="1">AX7+1</f>
-        <v>44450</v>
+        <v>45456</v>
       </c>
       <c r="AZ7" s="19">
         <f ca="1">AY7+1</f>
-        <v>44451</v>
+        <v>45457</v>
       </c>
       <c r="BA7" s="19">
         <f t="shared" ref="BA7:BE7" ca="1" si="1">AZ7+1</f>
-        <v>44452</v>
+        <v>45458</v>
       </c>
       <c r="BB7" s="19">
         <f t="shared" ca="1" si="1"/>
-        <v>44453</v>
+        <v>45459</v>
       </c>
       <c r="BC7" s="19">
         <f t="shared" ca="1" si="1"/>
-        <v>44454</v>
+        <v>45460</v>
       </c>
       <c r="BD7" s="19">
         <f t="shared" ca="1" si="1"/>
-        <v>44455</v>
+        <v>45461</v>
       </c>
       <c r="BE7" s="72">
         <f t="shared" ca="1" si="1"/>
-        <v>44456</v>
+        <v>45462</v>
       </c>
       <c r="BF7" s="19">
         <f ca="1">BE7+1</f>
-        <v>44457</v>
+        <v>45463</v>
       </c>
       <c r="BG7" s="19">
         <f ca="1">BF7+1</f>
-        <v>44458</v>
+        <v>45464</v>
       </c>
       <c r="BH7" s="19">
         <f t="shared" ref="BH7:BL7" ca="1" si="2">BG7+1</f>
-        <v>44459</v>
+        <v>45465</v>
       </c>
       <c r="BI7" s="19">
         <f t="shared" ca="1" si="2"/>
-        <v>44460</v>
+        <v>45466</v>
       </c>
       <c r="BJ7" s="19">
         <f t="shared" ca="1" si="2"/>
-        <v>44461</v>
+        <v>45467</v>
       </c>
       <c r="BK7" s="19">
         <f t="shared" ca="1" si="2"/>
-        <v>44462</v>
+        <v>45468</v>
       </c>
       <c r="BL7" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>44463</v>
+        <v>45469</v>
       </c>
       <c r="BM7" s="35"/>
     </row>
@@ -11247,7 +11305,7 @@
     <row r="9" spans="1:68" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="137" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C9" s="138" t="s">
         <v>7</v>
@@ -11267,23 +11325,23 @@
       <c r="H9" s="55"/>
       <c r="I9" s="43" t="str">
         <f t="shared" ref="I9:BL9" ca="1" si="3">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="J9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="K9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="L9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="M9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="N9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -11291,27 +11349,27 @@
       </c>
       <c r="O9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="P9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="Q9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="R9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="S9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="T9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="U9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -11319,27 +11377,27 @@
       </c>
       <c r="V9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="W9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="X9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="Y9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="Z9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AA9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="AB9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -11347,27 +11405,27 @@
       </c>
       <c r="AC9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="AD9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AE9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AF9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AG9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AH9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="AI9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -11375,27 +11433,27 @@
       </c>
       <c r="AJ9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="AK9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AL9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AM9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AN9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AO9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="AP9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -11403,27 +11461,27 @@
       </c>
       <c r="AQ9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="AR9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AS9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AT9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AU9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AV9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="AW9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -11431,27 +11489,27 @@
       </c>
       <c r="AX9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="AY9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AZ9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="BA9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BB9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="BC9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="BD9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -11459,27 +11517,27 @@
       </c>
       <c r="BE9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="BF9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="BG9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="BH9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BI9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="BJ9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="BK9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -11487,7 +11545,7 @@
       </c>
       <c r="BL9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="BM9" s="35"/>
     </row>
@@ -11560,10 +11618,14 @@
     <row r="11" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="139" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
+        <v>40</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>51</v>
+      </c>
       <c r="E11" s="25"/>
       <c r="F11" s="26"/>
       <c r="G11" s="27"/>
@@ -11798,32 +11860,29 @@
     <row r="12" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>8</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C12" s="24"/>
       <c r="D12" s="24" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="E12" s="25">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="F12" s="26">
-        <f ca="1">TODAY()</f>
-        <v>44407</v>
+        <v>45353</v>
       </c>
       <c r="G12" s="27">
         <v>3</v>
       </c>
       <c r="H12" s="22"/>
-      <c r="I12" s="54">
+      <c r="I12" s="54" t="str">
         <f ca="1">IF(AND($C12="Goal",I$7&gt;=$F12,I$7&lt;=$F12+$G12-1),2,IF(AND($C12="Milestone",I$7&gt;=$F12,I$7&lt;=$F12+$G12-1),1,""))</f>
-        <v>2</v>
-      </c>
-      <c r="J12" s="30">
-        <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v/>
+      </c>
+      <c r="J12" s="30" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
       <c r="K12" s="30" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -12046,16 +12105,17 @@
     <row r="13" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="28" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D13" s="24"/>
-      <c r="E13" s="25"/>
+      <c r="E13" s="25">
+        <v>1</v>
+      </c>
       <c r="F13" s="26">
-        <f ca="1">TODAY()+5</f>
-        <v>44412</v>
+        <v>45353</v>
       </c>
       <c r="G13" s="27">
         <v>1</v>
@@ -12077,9 +12137,9 @@
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="M13" s="30">
-        <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+      <c r="M13" s="30" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
       <c r="N13" s="30" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -12290,18 +12350,17 @@
     <row r="14" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="28" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="C14" s="24" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="25">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F14" s="26">
-        <f ca="1">F12-3</f>
-        <v>44404</v>
+        <v>45353</v>
       </c>
       <c r="G14" s="27">
         <v>10</v>
@@ -12536,16 +12595,17 @@
     <row r="15" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="28" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="C15" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
+      <c r="E15" s="25">
+        <v>1</v>
+      </c>
       <c r="F15" s="26">
-        <f ca="1">F12+20</f>
-        <v>44427</v>
+        <v>45353</v>
       </c>
       <c r="G15" s="27">
         <v>1</v>
@@ -12627,9 +12687,9 @@
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="AB15" s="30">
-        <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+      <c r="AB15" s="30" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
       <c r="AC15" s="30" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -12779,23 +12839,12 @@
     </row>
     <row r="16" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>13</v>
-      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="24"/>
-      <c r="E16" s="25">
-        <v>0.1</v>
-      </c>
-      <c r="F16" s="26">
-        <f ca="1">F12+6</f>
-        <v>44413</v>
-      </c>
-      <c r="G16" s="27">
-        <v>6</v>
-      </c>
+      <c r="E16" s="25"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="27"/>
       <c r="H16" s="22"/>
       <c r="I16" s="54" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -13025,245 +13074,150 @@
     </row>
     <row r="17" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
-      <c r="B17" s="139" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="27"/>
+      <c r="B17" s="137" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="138" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="138" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="138" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="138" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="138" t="s">
+        <v>25</v>
+      </c>
       <c r="H17" s="22"/>
-      <c r="I17" s="54" t="str">
-        <f t="shared" ca="1" si="8"/>
-        <v/>
-      </c>
-      <c r="J17" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="K17" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="L17" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="M17" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="N17" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="O17" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="P17" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="Q17" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="R17" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="S17" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="T17" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="U17" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="V17" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="W17" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="X17" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="Y17" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="Z17" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AA17" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AB17" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AC17" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AD17" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AE17" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AF17" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AG17" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AH17" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AI17" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AJ17" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AK17" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AL17" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AM17" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AN17" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AO17" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AP17" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AQ17" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AR17" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AS17" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AT17" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AU17" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AV17" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AW17" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AX17" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AY17" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AZ17" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BA17" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BB17" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BC17" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BD17" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BE17" s="30" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BF17" s="30" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BG17" s="30" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BH17" s="30" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BI17" s="30" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BJ17" s="30" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BK17" s="30" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BL17" s="30" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="54"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="30"/>
+      <c r="V17" s="30"/>
+      <c r="W17" s="30"/>
+      <c r="X17" s="54"/>
+      <c r="Y17" s="30"/>
+      <c r="Z17" s="30"/>
+      <c r="AA17" s="30"/>
+      <c r="AB17" s="54"/>
+      <c r="AC17" s="54"/>
+      <c r="AD17" s="30"/>
+      <c r="AE17" s="30"/>
+      <c r="AF17" s="30"/>
+      <c r="AG17" s="30"/>
+      <c r="AH17" s="54"/>
+      <c r="AI17" s="30"/>
+      <c r="AJ17" s="30"/>
+      <c r="AK17" s="30"/>
+      <c r="AL17" s="30"/>
+      <c r="AM17" s="54"/>
+      <c r="AN17" s="30"/>
+      <c r="AO17" s="30"/>
+      <c r="AP17" s="30"/>
+      <c r="AQ17" s="30"/>
+      <c r="AR17" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AS17" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT17" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AU17" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AV17" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AW17" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AX17" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AY17" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ17" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA17" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB17" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BC17" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BD17" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BE17" s="30" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BF17" s="30" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BG17" s="30" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BH17" s="30" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BI17" s="30" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BJ17" s="30" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BK17" s="30" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BL17" s="30" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#VALUE!</v>
       </c>
       <c r="BM17" s="31"/>
     </row>
     <row r="18" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="28" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="C18" s="24" t="s">
         <v>15</v>
@@ -13273,8 +13227,8 @@
         <v>0.6</v>
       </c>
       <c r="F18" s="26">
-        <f ca="1">F12+6</f>
-        <v>44413</v>
+        <f>F12+6</f>
+        <v>45359</v>
       </c>
       <c r="G18" s="27">
         <v>13</v>
@@ -13509,7 +13463,7 @@
     <row r="19" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="28" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="C19" s="24" t="s">
         <v>16</v>
@@ -13519,8 +13473,8 @@
         <v>0.5</v>
       </c>
       <c r="F19" s="26">
-        <f ca="1">F18+2</f>
-        <v>44415</v>
+        <f>F18+2</f>
+        <v>45361</v>
       </c>
       <c r="G19" s="27">
         <v>9</v>
@@ -13752,10 +13706,10 @@
       </c>
       <c r="BM19" s="31"/>
     </row>
-    <row r="20" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:65" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="28" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C20" s="24" t="s">
         <v>14</v>
@@ -13765,8 +13719,8 @@
         <v>0.33</v>
       </c>
       <c r="F20" s="26">
-        <f ca="1">F19+5</f>
-        <v>44420</v>
+        <f>F19+5</f>
+        <v>45366</v>
       </c>
       <c r="G20" s="27">
         <v>11</v>
@@ -14001,7 +13955,7 @@
     <row r="21" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="28" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="C21" s="24" t="s">
         <v>9</v>
@@ -14009,8 +13963,8 @@
       <c r="D21" s="24"/>
       <c r="E21" s="25"/>
       <c r="F21" s="26">
-        <f ca="1">F20+2</f>
-        <v>44422</v>
+        <f>F20+2</f>
+        <v>45368</v>
       </c>
       <c r="G21" s="27">
         <v>1</v>
@@ -14072,9 +14026,9 @@
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="W21" s="30">
-        <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+      <c r="W21" s="30" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
       <c r="X21" s="30" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -14244,19 +14198,12 @@
     </row>
     <row r="22" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
-      <c r="B22" s="28" t="s">
-        <v>2</v>
-      </c>
+      <c r="B22" s="28"/>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
       <c r="E22" s="25"/>
-      <c r="F22" s="26">
-        <f ca="1">F21+1</f>
-        <v>44423</v>
-      </c>
-      <c r="G22" s="27">
-        <v>24</v>
-      </c>
+      <c r="F22" s="26"/>
+      <c r="G22" s="27"/>
       <c r="H22" s="22"/>
       <c r="I22" s="54" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -14486,245 +14433,255 @@
     </row>
     <row r="23" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
-      <c r="B23" s="139" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="27"/>
+      <c r="B23" s="137" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="138" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="138" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="138" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="138" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="138" t="s">
+        <v>25</v>
+      </c>
       <c r="H23" s="22"/>
-      <c r="I23" s="54" t="str">
+      <c r="I23" s="54" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v/>
-      </c>
-      <c r="J23" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="K23" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="L23" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="M23" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="N23" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="O23" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="P23" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="Q23" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="R23" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="S23" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="T23" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="U23" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="V23" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="W23" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="X23" s="30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="Y23" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="Z23" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AA23" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AB23" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AC23" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AD23" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AE23" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AF23" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AG23" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AH23" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AI23" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AJ23" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AK23" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AL23" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AM23" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AN23" s="30" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AO23" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AP23" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AQ23" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AR23" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AS23" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AT23" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AU23" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AV23" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AW23" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AX23" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AY23" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AZ23" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BA23" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BB23" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BC23" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BD23" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BE23" s="30" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BF23" s="30" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BG23" s="30" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BH23" s="30" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BI23" s="30" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BJ23" s="30" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BK23" s="30" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BL23" s="30" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J23" s="30" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K23" s="30" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L23" s="30" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M23" s="30" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N23" s="30" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O23" s="30" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P23" s="30" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q23" s="30" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R23" s="30" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S23" s="30" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T23" s="30" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U23" s="30" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V23" s="30" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W23" s="30" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X23" s="30" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y23" s="30" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z23" s="30" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AA23" s="30" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AB23" s="30" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AC23" s="30" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AD23" s="30" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AE23" s="30" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AF23" s="30" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG23" s="30" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AH23" s="30" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AI23" s="30" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AJ23" s="30" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AK23" s="30" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL23" s="30" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM23" s="30" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN23" s="30" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO23" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP23" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ23" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR23" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AS23" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT23" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AU23" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AV23" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AW23" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AX23" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AY23" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ23" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA23" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB23" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BC23" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BD23" s="30" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BE23" s="30" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BF23" s="30" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BG23" s="30" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BH23" s="30" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BI23" s="30" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BJ23" s="30" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BK23" s="30" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BL23" s="30" t="e">
+        <f t="shared" ca="1" si="7"/>
+        <v>#VALUE!</v>
       </c>
       <c r="BM23" s="31"/>
     </row>
     <row r="24" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="28" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="C24" s="24" t="s">
         <v>16</v>
@@ -14732,8 +14689,8 @@
       <c r="D24" s="24"/>
       <c r="E24" s="25"/>
       <c r="F24" s="26">
-        <f ca="1">F12+15</f>
-        <v>44422</v>
+        <f>F12+15</f>
+        <v>45368</v>
       </c>
       <c r="G24" s="27">
         <v>4</v>
@@ -14976,8 +14933,8 @@
       <c r="D25" s="24"/>
       <c r="E25" s="25"/>
       <c r="F25" s="26">
-        <f ca="1">F24+3</f>
-        <v>44425</v>
+        <f>F24+3</f>
+        <v>45371</v>
       </c>
       <c r="G25" s="27">
         <v>14</v>
@@ -15220,8 +15177,8 @@
       <c r="D26" s="24"/>
       <c r="E26" s="25"/>
       <c r="F26" s="26">
-        <f ca="1">F25+15</f>
-        <v>44440</v>
+        <f>F25+15</f>
+        <v>45386</v>
       </c>
       <c r="G26" s="27">
         <v>6</v>
@@ -15464,8 +15421,8 @@
       <c r="D27" s="24"/>
       <c r="E27" s="25"/>
       <c r="F27" s="26">
-        <f ca="1">F21+22</f>
-        <v>44444</v>
+        <f>F21+22</f>
+        <v>45390</v>
       </c>
       <c r="G27" s="27">
         <v>3</v>
@@ -15615,17 +15572,17 @@
         <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
-      <c r="AS27" s="30">
-        <f t="shared" ca="1" si="9"/>
-        <v>2</v>
-      </c>
-      <c r="AT27" s="30">
-        <f t="shared" ca="1" si="9"/>
-        <v>2</v>
-      </c>
-      <c r="AU27" s="30">
-        <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+      <c r="AS27" s="30" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AT27" s="30" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AU27" s="30" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
       </c>
       <c r="AV27" s="30" t="str">
         <f t="shared" ca="1" si="9"/>
@@ -15708,8 +15665,8 @@
       <c r="D28" s="24"/>
       <c r="E28" s="25"/>
       <c r="F28" s="26">
-        <f ca="1">F16</f>
-        <v>44413</v>
+        <f>F16</f>
+        <v>0</v>
       </c>
       <c r="G28" s="27">
         <v>19</v>
@@ -15943,238 +15900,248 @@
     </row>
     <row r="29" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
-      <c r="B29" s="139" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="27"/>
+      <c r="B29" s="137" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="138" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="138" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="138" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="138" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="138" t="s">
+        <v>25</v>
+      </c>
       <c r="H29" s="22"/>
-      <c r="I29" s="54" t="str">
+      <c r="I29" s="54" t="e">
         <f t="shared" ref="I29:X35" ca="1" si="12">IF(AND($C29="Goal",I$7&gt;=$F29,I$7&lt;=$F29+$G29-1),2,IF(AND($C29="Milestone",I$7&gt;=$F29,I$7&lt;=$F29+$G29-1),1,""))</f>
-        <v/>
-      </c>
-      <c r="J29" s="30" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="K29" s="30" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="L29" s="30" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="M29" s="30" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="N29" s="30" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="O29" s="30" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="P29" s="30" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="Q29" s="30" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="R29" s="30" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="S29" s="30" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="T29" s="30" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="U29" s="30" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="V29" s="30" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="W29" s="30" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="X29" s="30" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="Y29" s="30" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="Z29" s="30" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AA29" s="30" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AB29" s="30" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AC29" s="30" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AD29" s="30" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AE29" s="30" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AF29" s="30" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AG29" s="30" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AH29" s="30" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AI29" s="30" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AJ29" s="30" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AK29" s="30" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AL29" s="30" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AM29" s="30" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AN29" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AO29" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AP29" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AQ29" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AR29" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AS29" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AT29" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AU29" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AV29" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AW29" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AX29" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AY29" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AZ29" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BA29" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BB29" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BC29" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BD29" s="30" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J29" s="30" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K29" s="30" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L29" s="30" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M29" s="30" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N29" s="30" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O29" s="30" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P29" s="30" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q29" s="30" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R29" s="30" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S29" s="30" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T29" s="30" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U29" s="30" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V29" s="30" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W29" s="30" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X29" s="30" t="e">
+        <f t="shared" ca="1" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y29" s="30" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z29" s="30" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AA29" s="30" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AB29" s="30" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AC29" s="30" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AD29" s="30" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AE29" s="30" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AF29" s="30" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG29" s="30" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AH29" s="30" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AI29" s="30" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AJ29" s="30" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AK29" s="30" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL29" s="30" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM29" s="30" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN29" s="30" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO29" s="30" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP29" s="30" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ29" s="30" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR29" s="30" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AS29" s="30" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT29" s="30" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AU29" s="30" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AV29" s="30" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AW29" s="30" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AX29" s="30" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AY29" s="30" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ29" s="30" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA29" s="30" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB29" s="30" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BC29" s="30" t="e">
+        <f t="shared" ca="1" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BD29" s="30" t="e">
         <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BE29" s="30" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="BE29" s="30" t="e">
         <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BF29" s="30" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="BF29" s="30" t="e">
         <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BG29" s="30" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="BG29" s="30" t="e">
         <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BH29" s="30" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="BH29" s="30" t="e">
         <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BI29" s="30" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="BI29" s="30" t="e">
         <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BJ29" s="30" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="BJ29" s="30" t="e">
         <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BK29" s="30" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="BK29" s="30" t="e">
         <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BL29" s="30" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="BL29" s="30" t="e">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="BM29" s="31"/>
     </row>
@@ -16187,8 +16154,8 @@
       <c r="D30" s="24"/>
       <c r="E30" s="25"/>
       <c r="F30" s="26">
-        <f ca="1">F27+3</f>
-        <v>44447</v>
+        <f>F27+3</f>
+        <v>45393</v>
       </c>
       <c r="G30" s="27">
         <v>15</v>
@@ -16429,8 +16396,8 @@
       <c r="D31" s="24"/>
       <c r="E31" s="25"/>
       <c r="F31" s="26">
-        <f ca="1">F30+14</f>
-        <v>44461</v>
+        <f>F30+14</f>
+        <v>45407</v>
       </c>
       <c r="G31" s="27">
         <v>5</v>
@@ -16673,8 +16640,8 @@
       <c r="D32" s="24"/>
       <c r="E32" s="25"/>
       <c r="F32" s="26">
-        <f ca="1">F31+42</f>
-        <v>44503</v>
+        <f>F31+42</f>
+        <v>45449</v>
       </c>
       <c r="G32" s="27">
         <v>1</v>
@@ -16820,9 +16787,9 @@
         <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
-      <c r="AR32" s="30" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
+      <c r="AR32" s="30">
+        <f t="shared" ca="1" si="9"/>
+        <v>1</v>
       </c>
       <c r="AS32" s="30" t="str">
         <f t="shared" ca="1" si="9"/>
@@ -17703,8 +17670,8 @@
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="S4:V4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E9:E36">
-    <cfRule type="dataBar" priority="5">
+  <conditionalFormatting sqref="E9:E16 E18:E22 E24:E28 E30:E36">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -17718,64 +17685,106 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL36">
-    <cfRule type="expression" dxfId="35" priority="1">
+    <cfRule type="expression" dxfId="35" priority="4">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="34" priority="4">
+    <cfRule type="expression" dxfId="34" priority="7">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BL6">
-    <cfRule type="expression" dxfId="33" priority="3">
+    <cfRule type="expression" dxfId="33" priority="6">
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BL6">
-    <cfRule type="expression" dxfId="32" priority="2">
+    <cfRule type="expression" dxfId="32" priority="5">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BL35">
-    <cfRule type="expression" dxfId="31" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="10" stopIfTrue="1">
       <formula>AND($C10="Low Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="11" stopIfTrue="1">
       <formula>AND($C10="High Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="12" stopIfTrue="1">
       <formula>AND($C10="On Track",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="13" stopIfTrue="1">
       <formula>AND($C10="Med Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="14" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:BL36">
-    <cfRule type="expression" dxfId="26" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="16" stopIfTrue="1">
       <formula>AND(#REF!="Low Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="17" stopIfTrue="1">
       <formula>AND(#REF!="High Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="18" stopIfTrue="1">
       <formula>AND(#REF!="On Track",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="19" stopIfTrue="1">
       <formula>AND(#REF!="Med Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="20" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{63A2BF1D-DFFF-44EB-B610-D0FD2814AC4D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{93E84C7F-E49C-4FB1-8567-853852A78CE2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{4BAEBD3A-1205-4511-853D-EBD5B57A7675}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="13">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C11" xr:uid="{DFFD23FF-9FE8-42D1-8B69-600D9BF05AA3}">
       <formula1>"Goal,Milestone,On Track, Low Risk, Med Risk, High Risk"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C35" xr:uid="{A2F07095-4C5B-4F26-9F4F-F9BCE27C6F57}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C16 C18:C22 C24:C28 C30:C35" xr:uid="{A2F07095-4C5B-4F26-9F4F-F9BCE27C6F57}">
       <formula1>"Goal,Milestone,On Track, Low Risk, Med Risk, High Risk"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="C7" xr:uid="{40D643B7-C378-45A2-A932-672EA7F96D14}">
@@ -17847,10 +17856,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E9:E36</xm:sqref>
+          <xm:sqref>E9:E16 E18:E22 E24:E28 E30:E36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="6" id="{C84307BC-4E4D-4989-9D21-88D6AEB0AFD2}">
+          <x14:cfRule type="iconSet" priority="9" id="{C84307BC-4E4D-4989-9D21-88D6AEB0AFD2}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -17869,7 +17878,7 @@
           <xm:sqref>I10:BL35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="12" id="{3EF75A3E-8286-4296-914E-C8F63A2E14FB}">
+          <x14:cfRule type="iconSet" priority="15" id="{3EF75A3E-8286-4296-914E-C8F63A2E14FB}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -17886,6 +17895,51 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>I36:BL36</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{63A2BF1D-DFFF-44EB-B610-D0FD2814AC4D}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E17</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{93E84C7F-E49C-4FB1-8567-853852A78CE2}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E23</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4BAEBD3A-1205-4511-853D-EBD5B57A7675}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E29</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -18211,7 +18265,7 @@
       </c>
       <c r="C6" s="90" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">IFERROR(IF(MIN(Milestones43524[Start])=0,TODAY(),B11(Milestones43524[Start])),TODAY())</f>
-        <v>44407</v>
+        <v>45414</v>
       </c>
       <c r="D6" s="91"/>
       <c r="E6" s="84"/>
@@ -18220,7 +18274,7 @@
       <c r="H6" s="84"/>
       <c r="I6" s="109" t="str">
         <f ca="1">TEXT(I7,"mmmm")</f>
-        <v>August</v>
+        <v>May</v>
       </c>
       <c r="J6" s="109"/>
       <c r="K6" s="109"/>
@@ -18260,7 +18314,7 @@
       <c r="AJ6" s="109"/>
       <c r="AK6" s="109" t="str">
         <f ca="1">IF(OR(TEXT(AK7,"mmmm")=AD6,TEXT(AK7,"mmmm")=W6,TEXT(AK7,"mmmm")=P6,TEXT(AK7,"mmmm")=I6),"",TEXT(AK7,"mmmm"))</f>
-        <v>September</v>
+        <v>June</v>
       </c>
       <c r="AL6" s="109"/>
       <c r="AM6" s="109"/>
@@ -18315,227 +18369,227 @@
       <c r="H7" s="94"/>
       <c r="I7" s="116">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>44412</v>
+        <v>45419</v>
       </c>
       <c r="J7" s="117">
         <f ca="1">I7+1</f>
-        <v>44413</v>
+        <v>45420</v>
       </c>
       <c r="K7" s="117">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>44414</v>
+        <v>45421</v>
       </c>
       <c r="L7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44415</v>
+        <v>45422</v>
       </c>
       <c r="M7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44416</v>
+        <v>45423</v>
       </c>
       <c r="N7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44417</v>
+        <v>45424</v>
       </c>
       <c r="O7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44418</v>
+        <v>45425</v>
       </c>
       <c r="P7" s="117">
         <f ca="1">O7+1</f>
-        <v>44419</v>
+        <v>45426</v>
       </c>
       <c r="Q7" s="117">
         <f ca="1">P7+1</f>
-        <v>44420</v>
+        <v>45427</v>
       </c>
       <c r="R7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44421</v>
+        <v>45428</v>
       </c>
       <c r="S7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44422</v>
+        <v>45429</v>
       </c>
       <c r="T7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44423</v>
+        <v>45430</v>
       </c>
       <c r="U7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44424</v>
+        <v>45431</v>
       </c>
       <c r="V7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44425</v>
+        <v>45432</v>
       </c>
       <c r="W7" s="117">
         <f ca="1">V7+1</f>
-        <v>44426</v>
+        <v>45433</v>
       </c>
       <c r="X7" s="117">
         <f ca="1">W7+1</f>
-        <v>44427</v>
+        <v>45434</v>
       </c>
       <c r="Y7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44428</v>
+        <v>45435</v>
       </c>
       <c r="Z7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44429</v>
+        <v>45436</v>
       </c>
       <c r="AA7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44430</v>
+        <v>45437</v>
       </c>
       <c r="AB7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44431</v>
+        <v>45438</v>
       </c>
       <c r="AC7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44432</v>
+        <v>45439</v>
       </c>
       <c r="AD7" s="117">
         <f ca="1">AC7+1</f>
-        <v>44433</v>
+        <v>45440</v>
       </c>
       <c r="AE7" s="117">
         <f ca="1">AD7+1</f>
-        <v>44434</v>
+        <v>45441</v>
       </c>
       <c r="AF7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44435</v>
+        <v>45442</v>
       </c>
       <c r="AG7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44436</v>
+        <v>45443</v>
       </c>
       <c r="AH7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44437</v>
+        <v>45444</v>
       </c>
       <c r="AI7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44438</v>
+        <v>45445</v>
       </c>
       <c r="AJ7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44439</v>
+        <v>45446</v>
       </c>
       <c r="AK7" s="117">
         <f ca="1">AJ7+1</f>
-        <v>44440</v>
+        <v>45447</v>
       </c>
       <c r="AL7" s="117">
         <f ca="1">AK7+1</f>
-        <v>44441</v>
+        <v>45448</v>
       </c>
       <c r="AM7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44442</v>
+        <v>45449</v>
       </c>
       <c r="AN7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44443</v>
+        <v>45450</v>
       </c>
       <c r="AO7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44444</v>
+        <v>45451</v>
       </c>
       <c r="AP7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44445</v>
+        <v>45452</v>
       </c>
       <c r="AQ7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44446</v>
+        <v>45453</v>
       </c>
       <c r="AR7" s="117">
         <f ca="1">AQ7+1</f>
-        <v>44447</v>
+        <v>45454</v>
       </c>
       <c r="AS7" s="117">
         <f ca="1">AR7+1</f>
-        <v>44448</v>
+        <v>45455</v>
       </c>
       <c r="AT7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44449</v>
+        <v>45456</v>
       </c>
       <c r="AU7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44450</v>
+        <v>45457</v>
       </c>
       <c r="AV7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44451</v>
+        <v>45458</v>
       </c>
       <c r="AW7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44452</v>
+        <v>45459</v>
       </c>
       <c r="AX7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44453</v>
+        <v>45460</v>
       </c>
       <c r="AY7" s="117">
         <f ca="1">AX7+1</f>
-        <v>44454</v>
+        <v>45461</v>
       </c>
       <c r="AZ7" s="117">
         <f ca="1">AY7+1</f>
-        <v>44455</v>
+        <v>45462</v>
       </c>
       <c r="BA7" s="117">
         <f t="shared" ref="BA7:BE7" ca="1" si="1">AZ7+1</f>
-        <v>44456</v>
+        <v>45463</v>
       </c>
       <c r="BB7" s="117">
         <f t="shared" ca="1" si="1"/>
-        <v>44457</v>
+        <v>45464</v>
       </c>
       <c r="BC7" s="117">
         <f t="shared" ca="1" si="1"/>
-        <v>44458</v>
+        <v>45465</v>
       </c>
       <c r="BD7" s="117">
         <f t="shared" ca="1" si="1"/>
-        <v>44459</v>
+        <v>45466</v>
       </c>
       <c r="BE7" s="118">
         <f t="shared" ca="1" si="1"/>
-        <v>44460</v>
+        <v>45467</v>
       </c>
       <c r="BF7" s="117">
         <f ca="1">BE7+1</f>
-        <v>44461</v>
+        <v>45468</v>
       </c>
       <c r="BG7" s="117">
         <f ca="1">BF7+1</f>
-        <v>44462</v>
+        <v>45469</v>
       </c>
       <c r="BH7" s="117">
         <f t="shared" ref="BH7:BL7" ca="1" si="2">BG7+1</f>
-        <v>44463</v>
+        <v>45470</v>
       </c>
       <c r="BI7" s="117">
         <f t="shared" ca="1" si="2"/>
-        <v>44464</v>
+        <v>45471</v>
       </c>
       <c r="BJ7" s="117">
         <f t="shared" ca="1" si="2"/>
-        <v>44465</v>
+        <v>45472</v>
       </c>
       <c r="BK7" s="117">
         <f t="shared" ca="1" si="2"/>
-        <v>44466</v>
+        <v>45473</v>
       </c>
       <c r="BL7" s="118">
         <f t="shared" ca="1" si="2"/>
-        <v>44467</v>
+        <v>45474</v>
       </c>
       <c r="BM7" s="99"/>
     </row>
@@ -18629,19 +18683,19 @@
       <c r="H9" s="105"/>
       <c r="I9" s="124" t="str">
         <f t="shared" ref="I9:BL9" ca="1" si="3">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="J9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="K9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="L9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="M9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -18649,27 +18703,27 @@
       </c>
       <c r="N9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="O9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="P9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="Q9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="R9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="S9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="T9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -18677,27 +18731,27 @@
       </c>
       <c r="U9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="V9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="W9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="X9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="Y9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="Z9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AA9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -18705,27 +18759,27 @@
       </c>
       <c r="AB9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AC9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AD9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="AE9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="AF9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AG9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AH9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -18733,27 +18787,27 @@
       </c>
       <c r="AI9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AJ9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AK9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="AL9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="AM9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AN9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AO9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -18761,27 +18815,27 @@
       </c>
       <c r="AP9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AQ9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AR9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="AS9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="AT9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AU9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AV9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -18789,27 +18843,27 @@
       </c>
       <c r="AW9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AX9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AY9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="AZ9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="BA9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="BB9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="BC9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -18817,27 +18871,27 @@
       </c>
       <c r="BD9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BE9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="BF9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="BG9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="BH9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="BI9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="BJ9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -18845,11 +18899,11 @@
       </c>
       <c r="BK9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BL9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="BM9" s="99"/>
     </row>
@@ -19173,7 +19227,7 @@
       </c>
       <c r="F12" s="69">
         <f ca="1">TODAY()</f>
-        <v>44407</v>
+        <v>45414</v>
       </c>
       <c r="G12" s="70">
         <v>3</v>
@@ -19417,7 +19471,7 @@
       <c r="E13" s="68"/>
       <c r="F13" s="69">
         <f ca="1">TODAY()+5</f>
-        <v>44412</v>
+        <v>45419</v>
       </c>
       <c r="G13" s="70">
         <v>1</v>
@@ -19663,7 +19717,7 @@
       </c>
       <c r="F14" s="69">
         <f ca="1">F12-3</f>
-        <v>44404</v>
+        <v>45411</v>
       </c>
       <c r="G14" s="70">
         <v>10</v>
@@ -19907,7 +19961,7 @@
       <c r="E15" s="68"/>
       <c r="F15" s="69">
         <f ca="1">F12+20</f>
-        <v>44427</v>
+        <v>45434</v>
       </c>
       <c r="G15" s="70">
         <v>1</v>
@@ -20153,7 +20207,7 @@
       </c>
       <c r="F16" s="69">
         <f ca="1">F12+6</f>
-        <v>44413</v>
+        <v>45420</v>
       </c>
       <c r="G16" s="70">
         <v>6</v>
@@ -20636,7 +20690,7 @@
       </c>
       <c r="F18" s="69">
         <f ca="1">F12+6</f>
-        <v>44413</v>
+        <v>45420</v>
       </c>
       <c r="G18" s="70">
         <v>13</v>
@@ -20882,7 +20936,7 @@
       </c>
       <c r="F19" s="69">
         <f ca="1">F18+2</f>
-        <v>44415</v>
+        <v>45422</v>
       </c>
       <c r="G19" s="70">
         <v>9</v>
@@ -21128,7 +21182,7 @@
       </c>
       <c r="F20" s="69">
         <f ca="1">F19+5</f>
-        <v>44420</v>
+        <v>45427</v>
       </c>
       <c r="G20" s="70">
         <v>11</v>
@@ -21372,7 +21426,7 @@
       <c r="E21" s="68"/>
       <c r="F21" s="69">
         <f ca="1">F20+2</f>
-        <v>44422</v>
+        <v>45429</v>
       </c>
       <c r="G21" s="70">
         <v>1</v>
@@ -21614,7 +21668,7 @@
       <c r="E22" s="68"/>
       <c r="F22" s="69">
         <f ca="1">F21+1</f>
-        <v>44423</v>
+        <v>45430</v>
       </c>
       <c r="G22" s="70">
         <v>24</v>
@@ -22095,7 +22149,7 @@
       <c r="E24" s="68"/>
       <c r="F24" s="69">
         <f ca="1">F12+15</f>
-        <v>44422</v>
+        <v>45429</v>
       </c>
       <c r="G24" s="70">
         <v>4</v>
@@ -22339,7 +22393,7 @@
       <c r="E25" s="68"/>
       <c r="F25" s="69">
         <f ca="1">F24+3</f>
-        <v>44425</v>
+        <v>45432</v>
       </c>
       <c r="G25" s="70">
         <v>14</v>
@@ -22583,7 +22637,7 @@
       <c r="E26" s="68"/>
       <c r="F26" s="69">
         <f ca="1">F25+15</f>
-        <v>44440</v>
+        <v>45447</v>
       </c>
       <c r="G26" s="70">
         <v>6</v>
@@ -22827,7 +22881,7 @@
       <c r="E27" s="68"/>
       <c r="F27" s="69">
         <f ca="1">F21+22</f>
-        <v>44444</v>
+        <v>45451</v>
       </c>
       <c r="G27" s="70">
         <v>3</v>
@@ -23071,7 +23125,7 @@
       <c r="E28" s="68"/>
       <c r="F28" s="69">
         <f ca="1">F16</f>
-        <v>44413</v>
+        <v>45420</v>
       </c>
       <c r="G28" s="70">
         <v>19</v>
@@ -23550,7 +23604,7 @@
       <c r="E30" s="68"/>
       <c r="F30" s="69">
         <f ca="1">F27+3</f>
-        <v>44447</v>
+        <v>45454</v>
       </c>
       <c r="G30" s="70">
         <v>15</v>
@@ -23792,7 +23846,7 @@
       <c r="E31" s="68"/>
       <c r="F31" s="69">
         <f ca="1">F30+14</f>
-        <v>44461</v>
+        <v>45468</v>
       </c>
       <c r="G31" s="70">
         <v>5</v>
@@ -24036,7 +24090,7 @@
       <c r="E32" s="68"/>
       <c r="F32" s="69">
         <f ca="1">F31+42</f>
-        <v>44503</v>
+        <v>45510</v>
       </c>
       <c r="G32" s="70">
         <v>1</v>
@@ -25256,6 +25310,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -25272,15 +25335,6 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25560,6 +25614,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -25567,14 +25629,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
     <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>